<commit_message>
resolucion counting in the amazon
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>fake-binary</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>counting-in-the-amazon</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -466,6 +471,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -483,6 +493,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -500,6 +515,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -517,6 +537,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -534,6 +559,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -551,6 +581,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -568,6 +603,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -585,6 +625,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -602,6 +647,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -619,6 +669,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -636,6 +691,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -653,6 +713,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -667,6 +732,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
@@ -687,6 +757,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -704,6 +779,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -721,6 +801,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -738,6 +823,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -755,6 +845,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -772,6 +867,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -789,6 +889,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -806,6 +911,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -823,6 +933,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -840,6 +955,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -857,6 +977,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -872,6 +997,11 @@
       <c r="C26" t="inlineStr">
         <is>
           <t>Good</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
resultado notas de clase
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -491,8 +491,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F2" t="b">
-        <v>0</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -521,8 +523,10 @@
           <t>No</t>
         </is>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -551,8 +555,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F4" t="b">
-        <v>0</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -581,8 +587,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F5" t="b">
-        <v>0</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -611,8 +619,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -641,8 +651,10 @@
           <t>No</t>
         </is>
       </c>
-      <c r="F7" t="b">
-        <v>0</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -671,8 +683,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F8" t="b">
-        <v>0</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -701,8 +715,10 @@
           <t>No</t>
         </is>
       </c>
-      <c r="F9" t="b">
-        <v>0</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -731,8 +747,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F10" t="b">
-        <v>0</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -761,8 +779,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F11" t="b">
-        <v>0</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -791,8 +811,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F12" t="b">
-        <v>0</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -821,8 +843,10 @@
           <t>No</t>
         </is>
       </c>
-      <c r="F13" t="b">
-        <v>0</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -851,8 +875,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F14" t="b">
-        <v>0</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -881,8 +907,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F15" t="b">
-        <v>0</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -911,8 +939,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F16" t="b">
-        <v>0</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -941,8 +971,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F17" t="b">
-        <v>0</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -971,8 +1003,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F18" t="b">
-        <v>0</v>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1001,8 +1035,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F19" t="b">
-        <v>0</v>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1031,8 +1067,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F20" t="b">
-        <v>0</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1061,8 +1099,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F21" t="b">
-        <v>0</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1091,8 +1131,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F22" t="b">
-        <v>0</v>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1121,8 +1163,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F23" t="b">
-        <v>0</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1151,8 +1195,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F24" t="b">
-        <v>0</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1181,8 +1227,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F25" t="b">
-        <v>0</v>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1211,8 +1259,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F26" t="b">
-        <v>0</v>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1241,8 +1291,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="F27" t="b">
-        <v>0</v>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ya funcina con smiley faces
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>tests-results</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>count-the-smiley-faces</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -496,6 +501,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -528,6 +538,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -560,6 +575,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -592,6 +612,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -621,6 +646,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
@@ -656,6 +686,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -688,6 +723,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -717,7 +757,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Good</t>
         </is>
       </c>
     </row>
@@ -752,6 +797,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -784,6 +834,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -816,6 +871,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -848,6 +908,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -880,6 +945,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -912,6 +982,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -944,6 +1019,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -976,6 +1056,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1005,6 +1090,11 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
@@ -1040,6 +1130,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1072,6 +1167,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1104,6 +1204,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1136,6 +1241,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1168,6 +1278,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1197,6 +1312,11 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
@@ -1232,6 +1352,11 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1264,6 +1389,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1292,6 +1422,11 @@
         </is>
       </c>
       <c r="F27" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>Good</t>
         </is>

</xml_diff>

<commit_message>
next happy year puntuacion
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -521,8 +521,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -566,8 +568,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I3" t="b">
-        <v>0</v>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -611,8 +615,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I4" t="b">
-        <v>0</v>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -656,8 +662,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I5" t="b">
-        <v>0</v>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -701,8 +709,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I6" t="b">
-        <v>0</v>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -746,8 +756,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I7" t="b">
-        <v>0</v>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -791,8 +803,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I8" t="b">
-        <v>0</v>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -836,8 +850,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I9" t="b">
-        <v>0</v>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -881,8 +897,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I10" t="b">
-        <v>0</v>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -926,8 +944,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I11" t="b">
-        <v>0</v>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -971,8 +991,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I12" t="b">
-        <v>0</v>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -1016,8 +1038,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I13" t="b">
-        <v>0</v>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1061,8 +1085,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I14" t="b">
-        <v>0</v>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1106,8 +1132,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I15" t="b">
-        <v>0</v>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1151,8 +1179,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I16" t="b">
-        <v>0</v>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1196,8 +1226,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I17" t="b">
-        <v>0</v>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1241,8 +1273,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I18" t="b">
-        <v>0</v>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1286,8 +1320,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I19" t="b">
-        <v>0</v>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1331,8 +1367,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I20" t="b">
-        <v>0</v>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1376,8 +1414,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I21" t="b">
-        <v>0</v>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1421,8 +1461,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I22" t="b">
-        <v>0</v>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1466,8 +1508,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I23" t="b">
-        <v>0</v>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1511,8 +1555,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I24" t="b">
-        <v>0</v>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1556,8 +1602,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I25" t="b">
-        <v>0</v>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1601,8 +1649,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I26" t="b">
-        <v>0</v>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1646,8 +1696,10 @@
           <t>Good</t>
         </is>
       </c>
-      <c r="I27" t="b">
-        <v>0</v>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadido pete y cambio orden alumnos
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,11 +479,16 @@
           <t>see-you-next-happy-year</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>pete-the-baker</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>FerZZ</t>
+          <t>a_romegar</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -525,12 +530,15 @@
         <is>
           <t>Good</t>
         </is>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>juanchovpa</t>
+          <t>Afidalgo-fmm</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -550,12 +558,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -570,29 +578,32 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Juanpda</t>
+          <t>AnaWalsh</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -602,7 +613,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -619,12 +630,15 @@
         <is>
           <t>Good</t>
         </is>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>daniela-arias</t>
+          <t>Andrestart</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -639,7 +653,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -649,7 +663,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -666,6 +680,9 @@
         <is>
           <t>Good</t>
         </is>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -714,16 +731,19 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>silviarico</t>
+          <t>beatrizsp</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -733,17 +753,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -760,12 +780,15 @@
         <is>
           <t>No</t>
         </is>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>EduardoRivera_98</t>
+          <t>bvispo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -790,7 +813,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -805,14 +828,17 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Good</t>
-        </is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>LuisSerranoCerame</t>
+          <t>Carlosleono</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -832,7 +858,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -854,12 +880,15 @@
         <is>
           <t>Good</t>
         </is>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>mariaperezdeayalas</t>
+          <t>Danihelguera</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -884,7 +913,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -899,14 +928,17 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>NicolasPce</t>
+          <t>EduardoRivera_98</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -936,7 +968,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -948,12 +980,15 @@
         <is>
           <t>Good</t>
         </is>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>bvispo</t>
+          <t>elliotesp</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -978,12 +1013,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -995,12 +1030,15 @@
         <is>
           <t>No</t>
         </is>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>mariadelas</t>
+          <t>sinatxe</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1020,7 +1058,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1040,14 +1078,17 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>a_romegar</t>
+          <t>FerZZ</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1089,12 +1130,15 @@
         <is>
           <t>Good</t>
         </is>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Roblak96</t>
+          <t>Pnat1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1109,7 +1153,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1119,12 +1163,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1134,19 +1178,22 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>LydiaAR</t>
+          <t>Juanpda</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1156,7 +1203,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1166,7 +1213,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1181,14 +1228,17 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>beatrizsp</t>
+          <t>juanchovpa</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1203,12 +1253,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1230,12 +1280,15 @@
         <is>
           <t>No</t>
         </is>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>elliotesp</t>
+          <t>LuisSerranoCerame</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1255,7 +1308,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1275,14 +1328,17 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Carlosleono</t>
+          <t>LydiaAR</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1297,7 +1353,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1307,12 +1363,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1322,14 +1378,17 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Good</t>
-        </is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>pedromartinezleis</t>
+          <t>mariaperezdeayalas</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1354,7 +1413,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1369,14 +1428,17 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Good</t>
-        </is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Danihelguera</t>
+          <t>mariadelas</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1396,7 +1458,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1416,14 +1478,17 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Good</t>
-        </is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>sinatxe</t>
+          <t>NicolasPce</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1465,12 +1530,15 @@
         <is>
           <t>Good</t>
         </is>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Andrestart</t>
+          <t>pedromartinezleis</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1510,14 +1578,17 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Pnat1</t>
+          <t>Roblak96</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1532,7 +1603,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1542,12 +1613,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1557,19 +1628,22 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Good</t>
-        </is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>TheIronhidex</t>
+          <t>silviarico</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1584,7 +1658,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1604,14 +1678,17 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Good</t>
-        </is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>AnaWalsh</t>
+          <t>TheIronhidex</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1621,12 +1698,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1636,12 +1713,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1651,14 +1728,17 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Afidalgo-fmm</t>
+          <t>daniela-arias</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1673,7 +1753,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1683,7 +1763,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1698,8 +1778,11 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadido sorting by bits
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,11 @@
           <t>decode-the-morse-code</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>sorting-by-bits</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -566,6 +571,9 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -633,6 +641,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -700,6 +711,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -767,6 +781,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -834,6 +851,9 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -901,6 +921,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -968,6 +991,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1035,6 +1061,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1102,6 +1131,9 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1169,6 +1201,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1236,6 +1271,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1303,6 +1341,9 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="N13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1370,6 +1411,9 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="N14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1437,6 +1481,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1504,6 +1551,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N16" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1571,6 +1621,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1638,6 +1691,9 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="N18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1705,6 +1761,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1772,6 +1831,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N20" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1839,6 +1901,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1906,6 +1971,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N22" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1973,6 +2041,9 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="N23" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -2040,6 +2111,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N24" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -2107,6 +2181,9 @@
           <t>No</t>
         </is>
       </c>
+      <c r="N25" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -2174,6 +2251,9 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="N26" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -2240,6 +2320,9 @@
         <is>
           <t>No</t>
         </is>
+      </c>
+      <c r="N27" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>